<commit_message>
fix: Rerun the MALDI metadata reharmonization procedure
</commit_message>
<xml_diff>
--- a/metadata/maldi/todo/TTD - Pacific Northwest National Laboratory (MALDI).xlsx
+++ b/metadata/maldi/todo/TTD - Pacific Northwest National Laboratory (MALDI).xlsx
@@ -13,7 +13,7 @@
     <sheet name="Invalid Input Pattern" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Standard Value'!$A$1:$E$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Standard Value'!$A$1:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Missing Required Value'!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Invalid Input Pattern'!$A$1:$F$2</definedName>
   </definedNames>
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,20 +441,15 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Negative ion mode</t>
+          <t>MS1</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>MS1</t>
+          <t>2,5-DHB (2,5-Dihydroxybenzoic acid)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
-        <is>
-          <t>2,5-DHB (2,5-Dihydroxybenzoic acid)</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
         <is>
           <t>hour</t>
         </is>
@@ -473,20 +468,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Positive ion mode</t>
+          <t>MS3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MS3</t>
+          <t>NEDC (N-(1-naphthyl) ethylenediamine dihydrochloride)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
-        <is>
-          <t>NEDC (N-(1-naphthyl) ethylenediamine dihydrochloride)</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
         <is>
           <t>month</t>
         </is>
@@ -505,20 +495,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Negative and positive ion mode</t>
+          <t>MS2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MS2</t>
+          <t>SA (sinapic acid)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
-        <is>
-          <t>SA (sinapic acid)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
         <is>
           <t>year</t>
         </is>
@@ -535,12 +520,12 @@
           <t>SLIM</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>DAN (1,5-diaminonapthalene)</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
-        <is>
-          <t>DAN (1,5-diaminonapthalene)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
         <is>
           <t>day</t>
         </is>
@@ -557,12 +542,12 @@
           <t>TIMS</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2,5-DHA (2,5-dihydroxyacetophenone)</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
-        <is>
-          <t>2,5-DHA (2,5-dihydroxyacetophenone)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
         <is>
           <t>minute</t>
         </is>
@@ -579,7 +564,7 @@
           <t>FAIMS</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>9-AA (9-aminoacridine)</t>
         </is>
@@ -591,7 +576,7 @@
           <t>EVOS M7000</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>CHCA (alpha-cyano-4-hydroxy-cinnamic acid)</t>
         </is>
@@ -603,7 +588,7 @@
           <t>NovaSeq X</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>DMACA (4-(dimethylamino)cinnamic acid)</t>
         </is>
@@ -1103,7 +1088,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1188,12 +1173,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>mass_analysis_polarity</t>
+          <t>ms_scan_mode</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>positive ion mode</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -1211,14 +1196,10 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ms_scan_mode</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
+          <t>preparation_matrix</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
@@ -1226,28 +1207,9 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>HBM666.BBVZ.767</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>preparation_matrix</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM666.BBVZ.767</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E6"/>
-  <dataValidations count="5">
+  <autoFilter ref="A1:E5"/>
+  <dataValidations count="4">
     <dataValidation sqref="D2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
       <formula1>_validation_data!$A$1:$A$77</formula1>
     </dataValidation>
@@ -1258,10 +1220,7 @@
       <formula1>_validation_data!$C$1:$C$3</formula1>
     </dataValidation>
     <dataValidation sqref="D5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$D$1:$D$3</formula1>
-    </dataValidation>
-    <dataValidation sqref="D6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$E$1:$E$8</formula1>
+      <formula1>_validation_data!$D$1:$D$8</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1380,10 +1339,10 @@
   <autoFilter ref="A1:D5"/>
   <dataValidations count="2">
     <dataValidation sqref="C3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$E$1:$E$8</formula1>
+      <formula1>_validation_data!$D$1:$D$8</formula1>
     </dataValidation>
     <dataValidation sqref="C4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$F$1:$F$5</formula1>
+      <formula1>_validation_data!$E$1:$E$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: Rerun reharmonization pipeline for MALDI
</commit_message>
<xml_diff>
--- a/metadata/maldi/todo/TTD - Pacific Northwest National Laboratory (MALDI).xlsx
+++ b/metadata/maldi/todo/TTD - Pacific Northwest National Laboratory (MALDI).xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,425 +653,453 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>timsTOF Pro 2</t>
+          <t>Opera Phenix Plus HCS</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Q Exactive UHMR</t>
+          <t>timsTOF Pro 2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Q Exactive</t>
+          <t>Q Exactive UHMR</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>timsTOF SCP</t>
+          <t>Q Exactive</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Zyla 4.2 sCMOS</t>
+          <t>timsTOF SCP</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Helios</t>
+          <t>Zyla 4.2 sCMOS</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>uScopeHXII-20</t>
+          <t>Helios</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Custom: Multiphoton</t>
+          <t>uScopeHXII-20</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>QTRAP 5500</t>
+          <t>Orbitrap Fusion Tribrid</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>timsTOF Ultra</t>
+          <t>Custom: Multiphoton</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BZ-X800</t>
+          <t>QTRAP 5500</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CyTOF 2</t>
+          <t>timsTOF Ultra</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>G4X Spatial Sequencer</t>
+          <t>BZ-X800</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>NextSeq 500</t>
+          <t>CyTOF 2</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>NanoZoomer S360</t>
+          <t>G4X Spatial Sequencer</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Hyperion Imaging System</t>
+          <t>NextSeq 500</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>NovaSeq X Plus</t>
+          <t>NanoZoomer S360</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CyTOF XT</t>
+          <t>Hyperion Imaging System</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>NanoZoomer-SQ</t>
+          <t>NovaSeq X Plus</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>NextSeq 550</t>
+          <t>CyTOF XT</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Axio Zoom.V16</t>
+          <t>NanoZoomer-SQ</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Digital Spatial Profiler</t>
+          <t>NextSeq 550</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>timsTOF FleX</t>
+          <t>Axio Zoom.V16</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>timsTOF FleX MALDI-2</t>
+          <t>Digital Spatial Profiler</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>NanoZoomer S210</t>
+          <t>timsTOF FleX</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>BZ-X810</t>
+          <t>timsTOF FleX MALDI-2</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Axio Observer 7</t>
+          <t>NanoZoomer S210</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Cytek Northern Lights</t>
+          <t>BZ-X810</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>IN Cell Analyzer 2200</t>
+          <t>Axio Observer 7</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>timsTOF HT</t>
+          <t>Cytek Northern Lights</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>PhenoImager Fusion</t>
+          <t>Zeiss LightSheet Z.1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>DM6 B</t>
+          <t>IN Cell Analyzer 2200</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Phenocycler-Fusion 2.0</t>
+          <t>timsTOF HT</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Aperio CS2</t>
+          <t>PhenoImager Fusion</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Orbitrap Fusion Lumos Tribrid</t>
+          <t>DM6 B</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Resolve Biosciences Molecular Cartography</t>
+          <t>Phenocycler-Fusion 2.0</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>MALDI timsTOF Flex Prototype</t>
+          <t>Aperio CS2</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TissueScope LE Slide Scanner</t>
+          <t>Orbitrap Fusion Lumos Tribrid</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>VS200 Slide Scanner</t>
+          <t>Resolve Biosciences Molecular Cartography</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Axio Observer 5</t>
+          <t>MALDI timsTOF Flex Prototype</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Axio Observer 3</t>
+          <t>TissueScope LE Slide Scanner</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>HiSeq 2500</t>
+          <t>VS200 Slide Scanner</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Orbitrap Eclipse Tribrid</t>
+          <t>Axio Observer 5</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Cell DIVE</t>
+          <t>Axio Observer 3</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MERSCOPE</t>
+          <t>HiSeq 2500</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>NextSeq 2000</t>
+          <t>Orbitrap Eclipse Tribrid</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>NovaSeq 6000</t>
+          <t>Cell DIVE</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>In-House</t>
+          <t>MERSCOPE</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>HiSeq 4000</t>
+          <t>NextSeq 2000</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>solariX</t>
+          <t>NovaSeq 6000</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Panoramic 150 Digital Scanner</t>
+          <t>In-House</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Aperio AT2</t>
+          <t>HiSeq 4000</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MIBIscope</t>
+          <t>solariX</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Biomark HD</t>
+          <t>Panoramic 150 Digital Scanner</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>NanoZoomer S60</t>
+          <t>Aperio AT2</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>CosMx Spatial Molecular Imager</t>
+          <t>MIBIscope</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MERSCOPE Ultra</t>
+          <t>SYNAPT G2-Si</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Axio Scan.Z1</t>
+          <t>Biomark HD</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Juno System</t>
+          <t>NanoZoomer S60</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Q Exactive HF</t>
+          <t>CosMx Spatial Molecular Imager</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
+        <is>
+          <t>MERSCOPE Ultra</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Axio Scan.Z1</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Juno System</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Q Exactive HF</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
         <is>
           <t>Xenium Analyzer</t>
         </is>
@@ -1211,7 +1239,7 @@
   <autoFilter ref="A1:E5"/>
   <dataValidations count="4">
     <dataValidation sqref="D2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$A$1:$A$77</formula1>
+      <formula1>_validation_data!$A$1:$A$81</formula1>
     </dataValidation>
     <dataValidation sqref="D3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
       <formula1>_validation_data!$B$1:$B$6</formula1>

</xml_diff>